<commit_message>
Removed obsolete files; added demo files for section #5, added data source tabs in each Excel file
</commit_message>
<xml_diff>
--- a/Section 2/2. Making a perfect line chart - Excel demo file.xlsx
+++ b/Section 2/2. Making a perfect line chart - Excel demo file.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikit\OneDrive\Documents\Courses\Perfect charts in Excel\2. Making a perfect line chart\2.2. - demo in excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikit\OneDrive\Documents\Courses\Perfect charts in Excel\Perfect-Excel-Charts\Section 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="235" documentId="8_{099F6B43-4BF7-4F4E-8445-3A5AB0D67290}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{4829805F-FAEF-4B52-8DE5-509B125ADF74}"/>
+  <xr:revisionPtr revIDLastSave="244" documentId="8_{099F6B43-4BF7-4F4E-8445-3A5AB0D67290}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{EE991A8E-59B6-4D9C-B771-14AC2272A5A2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24300" windowHeight="13710" activeTab="1" xr2:uid="{9B489133-FDDD-4F7B-8715-7C182468B235}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24300" windowHeight="13710" activeTab="2" xr2:uid="{9B489133-FDDD-4F7B-8715-7C182468B235}"/>
   </bookViews>
   <sheets>
     <sheet name="Normal line chart" sheetId="2" r:id="rId1"/>
     <sheet name="Stepped line chart" sheetId="4" r:id="rId2"/>
+    <sheet name="Sources" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Italy</t>
   </si>
@@ -35,6 +36,24 @@
   </si>
   <si>
     <t>France</t>
+  </si>
+  <si>
+    <t>Unemployment data</t>
+  </si>
+  <si>
+    <t>https://data.worldbank.org/indicator/SL.UEM.TOTL.NE.ZS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDP data: </t>
+  </si>
+  <si>
+    <t>https://data.worldbank.org/indicator/NY.GDP.MKTP.KD</t>
+  </si>
+  <si>
+    <t>https://www.coca-colacompany.com/content/dam/journey/us/en/private/fileassets/pdf/2018/TCCCAR17.pdf</t>
+  </si>
+  <si>
+    <t>Coca-Cola 2018 annual report</t>
   </si>
 </sst>
 </file>
@@ -7023,9 +7042,9 @@
       <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -7036,7 +7055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B3" s="3">
         <v>1970</v>
       </c>
@@ -7047,7 +7066,7 @@
         <v>2.4200000762939503E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B4" s="3">
         <v>1971</v>
       </c>
@@ -7058,7 +7077,7 @@
         <v>2.6700000762939501E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B5" s="3">
         <v>1972</v>
       </c>
@@ -7069,7 +7088,7 @@
         <v>2.7699999809265102E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B6" s="3">
         <v>1973</v>
       </c>
@@ -7080,7 +7099,7 @@
         <v>2.69000005722046E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B7" s="3">
         <v>1974</v>
       </c>
@@ -7091,7 +7110,7 @@
         <v>2.85999989509583E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B8" s="3">
         <v>1975</v>
       </c>
@@ -7102,7 +7121,7 @@
         <v>4.07999992370605E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B9" s="3">
         <v>1976</v>
       </c>
@@ -7113,7 +7132,7 @@
         <v>4.4699997901916505E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B10" s="3">
         <v>1977</v>
       </c>
@@ -7122,7 +7141,7 @@
         <v>5.0100002288818404E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B11" s="3">
         <v>1978</v>
       </c>
@@ -7133,7 +7152,7 @@
         <v>5.2699999809265104E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B12" s="3">
         <v>1979</v>
       </c>
@@ -7144,7 +7163,7 @@
         <v>6.0300002098083498E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B13" s="3">
         <v>1980</v>
       </c>
@@ -7155,7 +7174,7 @@
         <v>6.4200000762939496E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B14" s="3">
         <v>1981</v>
       </c>
@@ -7164,7 +7183,7 @@
         <v>7.5399999618530306E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B15" s="3">
         <v>1982</v>
       </c>
@@ -7175,7 +7194,7 @@
         <v>8.1999998092651405E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B16" s="3">
         <v>1983</v>
       </c>
@@ -7186,7 +7205,7 @@
         <v>7.9200000762939496E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B17" s="3">
         <v>1984</v>
       </c>
@@ -7197,7 +7216,7 @@
         <v>9.5299997329711894E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B18" s="3">
         <v>1985</v>
       </c>
@@ -7208,7 +7227,7 @@
         <v>0.10260000228881801</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B19" s="3">
         <v>1986</v>
       </c>
@@ -7219,7 +7238,7 @@
         <v>0.102299995422363</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B20" s="3">
         <v>1987</v>
       </c>
@@ -7230,7 +7249,7 @@
         <v>0.107399997711182</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B21" s="3">
         <v>1988</v>
       </c>
@@ -7241,7 +7260,7 @@
         <v>0.10180000305175801</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B22" s="3">
         <v>1989</v>
       </c>
@@ -7252,7 +7271,7 @@
         <v>9.6199998855590801E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B23" s="3">
         <v>1990</v>
       </c>
@@ -7263,7 +7282,7 @@
         <v>9.3400001525878906E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B24" s="3">
         <v>1991</v>
       </c>
@@ -7274,7 +7293,7 @@
         <v>9.1300001144409199E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B25" s="3">
         <v>1992</v>
       </c>
@@ -7285,7 +7304,7 @@
         <v>0.101300001144409</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B26" s="3">
         <v>1993</v>
       </c>
@@ -7296,7 +7315,7 @@
         <v>0.11199999809265099</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B27" s="3">
         <v>1994</v>
       </c>
@@ -7307,7 +7326,7 @@
         <v>0.12460000038147</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B28" s="3">
         <v>1995</v>
       </c>
@@ -7318,7 +7337,7 @@
         <v>0.118400001525879</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B29" s="3">
         <v>1996</v>
       </c>
@@ -7329,7 +7348,7 @@
         <v>0.12369999885559099</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B30" s="3">
         <v>1997</v>
       </c>
@@ -7340,7 +7359,7 @@
         <v>0.12359999656677199</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B31" s="3">
         <v>1998</v>
       </c>
@@ -7351,7 +7370,7 @@
         <v>0.118800001144409</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B32" s="3">
         <v>1999</v>
       </c>
@@ -7362,7 +7381,7 @@
         <v>0.11789999961853001</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B33" s="3">
         <v>2000</v>
       </c>
@@ -7373,7 +7392,7 @@
         <v>0.10060000419616699</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B34" s="3">
         <v>2001</v>
       </c>
@@ -7384,7 +7403,7 @@
         <v>8.819999694824221E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B35" s="3">
         <v>2002</v>
       </c>
@@ -7395,7 +7414,7 @@
         <v>8.9499998092651398E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B36" s="3">
         <v>2003</v>
       </c>
@@ -7406,7 +7425,7 @@
         <v>8.1499996185302695E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B37" s="3">
         <v>2004</v>
       </c>
@@ -7417,7 +7436,7 @@
         <v>8.5200004577636698E-2</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B38" s="3">
         <v>2005</v>
       </c>
@@ -7428,7 +7447,7 @@
         <v>8.5000000000000006E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B39" s="3">
         <v>2006</v>
       </c>
@@ -7439,7 +7458,7 @@
         <v>8.4499998092651407E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B40" s="3">
         <v>2007</v>
       </c>
@@ -7450,7 +7469,7 @@
         <v>7.6599998474121106E-2</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B41" s="3">
         <v>2008</v>
       </c>
@@ -7461,7 +7480,7 @@
         <v>7.0599999427795407E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B42" s="3">
         <v>2009</v>
       </c>
@@ -7472,7 +7491,7 @@
         <v>8.7399997711181607E-2</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B43" s="3">
         <v>2010</v>
       </c>
@@ -7483,7 +7502,7 @@
         <v>8.8699998855590809E-2</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B44" s="3">
         <v>2011</v>
       </c>
@@ -7494,7 +7513,7 @@
         <v>8.8100004196166995E-2</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B45" s="3">
         <v>2012</v>
       </c>
@@ -7505,7 +7524,7 @@
         <v>9.3999996185302692E-2</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B46" s="3">
         <v>2013</v>
       </c>
@@ -7516,7 +7535,7 @@
         <v>9.92000007629395E-2</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B47" s="3">
         <v>2014</v>
       </c>
@@ -7527,7 +7546,7 @@
         <v>0.10300000190734901</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B48" s="3">
         <v>2015</v>
       </c>
@@ -7538,7 +7557,7 @@
         <v>0.103599996566772</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B49" s="3">
         <v>2016</v>
       </c>
@@ -7559,13 +7578,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF08B8C-FAFE-49F2-9D53-562761FB275C}">
   <dimension ref="B2:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -7578,7 +7597,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B3" s="4">
         <v>25934</v>
       </c>
@@ -7589,7 +7608,7 @@
         <v>2.4200000762939503E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B4" s="4">
         <v>26299</v>
       </c>
@@ -7600,7 +7619,7 @@
         <v>2.6700000762939501E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B5" s="4">
         <v>26665</v>
       </c>
@@ -7611,7 +7630,7 @@
         <v>2.7699999809265102E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B6" s="4">
         <v>27030</v>
       </c>
@@ -7622,7 +7641,7 @@
         <v>2.69000005722046E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B7" s="4">
         <v>27395</v>
       </c>
@@ -7633,7 +7652,7 @@
         <v>2.85999989509583E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B8" s="4">
         <v>27760</v>
       </c>
@@ -7644,7 +7663,7 @@
         <v>4.07999992370605E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B9" s="4">
         <v>28126</v>
       </c>
@@ -7655,7 +7674,7 @@
         <v>4.4699997901916505E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B10" s="4">
         <v>28491</v>
       </c>
@@ -7664,7 +7683,7 @@
         <v>5.0100002288818404E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B11" s="4">
         <v>28856</v>
       </c>
@@ -7675,7 +7694,7 @@
         <v>5.2699999809265104E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B12" s="4">
         <v>29221</v>
       </c>
@@ -7686,7 +7705,7 @@
         <v>6.0300002098083498E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B13" s="4">
         <v>29587</v>
       </c>
@@ -7697,7 +7716,7 @@
         <v>6.4200000762939496E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B14" s="4">
         <v>29952</v>
       </c>
@@ -7706,7 +7725,7 @@
         <v>7.5399999618530306E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B15" s="4">
         <v>30317</v>
       </c>
@@ -7717,7 +7736,7 @@
         <v>8.1999998092651405E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B16" s="4">
         <v>30682</v>
       </c>
@@ -7728,7 +7747,7 @@
         <v>7.9200000762939496E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B17" s="4">
         <v>31048</v>
       </c>
@@ -7739,7 +7758,7 @@
         <v>9.5299997329711894E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B18" s="4">
         <v>31413</v>
       </c>
@@ -7750,7 +7769,7 @@
         <v>0.10260000228881801</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B19" s="4">
         <v>31778</v>
       </c>
@@ -7761,7 +7780,7 @@
         <v>0.102299995422363</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B20" s="4">
         <v>32143</v>
       </c>
@@ -7772,7 +7791,7 @@
         <v>0.107399997711182</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B21" s="4">
         <v>32509</v>
       </c>
@@ -7783,7 +7802,7 @@
         <v>0.10180000305175801</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B22" s="4">
         <v>32874</v>
       </c>
@@ -7794,7 +7813,7 @@
         <v>9.6199998855590801E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B23" s="4">
         <v>33239</v>
       </c>
@@ -7805,7 +7824,7 @@
         <v>9.3400001525878906E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B24" s="4">
         <v>33604</v>
       </c>
@@ -7816,7 +7835,7 @@
         <v>9.1300001144409199E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B25" s="4">
         <v>33970</v>
       </c>
@@ -7827,7 +7846,7 @@
         <v>0.101300001144409</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B26" s="4">
         <v>34335</v>
       </c>
@@ -7838,7 +7857,7 @@
         <v>0.11199999809265099</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B27" s="4">
         <v>34700</v>
       </c>
@@ -7849,7 +7868,7 @@
         <v>0.12460000038147</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B28" s="4">
         <v>35065</v>
       </c>
@@ -7860,7 +7879,7 @@
         <v>0.118400001525879</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B29" s="4">
         <v>35431</v>
       </c>
@@ -7871,7 +7890,7 @@
         <v>0.12369999885559099</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B30" s="4">
         <v>35796</v>
       </c>
@@ -7882,7 +7901,7 @@
         <v>0.12359999656677199</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B31" s="4">
         <v>36161</v>
       </c>
@@ -7893,7 +7912,7 @@
         <v>0.118800001144409</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B32" s="4">
         <v>36526</v>
       </c>
@@ -7904,7 +7923,7 @@
         <v>0.11789999961853001</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B33" s="4">
         <v>36892</v>
       </c>
@@ -7915,7 +7934,7 @@
         <v>0.10060000419616699</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B34" s="4">
         <v>37257</v>
       </c>
@@ -7926,7 +7945,7 @@
         <v>8.819999694824221E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B35" s="4">
         <v>37622</v>
       </c>
@@ -7937,7 +7956,7 @@
         <v>8.9499998092651398E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B36" s="4">
         <v>37987</v>
       </c>
@@ -7948,7 +7967,7 @@
         <v>8.1499996185302695E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B37" s="4">
         <v>38353</v>
       </c>
@@ -7959,7 +7978,7 @@
         <v>8.5200004577636698E-2</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B38" s="4">
         <v>38718</v>
       </c>
@@ -7970,7 +7989,7 @@
         <v>8.5000000000000006E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B39" s="4">
         <v>39083</v>
       </c>
@@ -7981,7 +8000,7 @@
         <v>8.4499998092651407E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B40" s="4">
         <v>39448</v>
       </c>
@@ -7992,7 +8011,7 @@
         <v>7.6599998474121106E-2</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B41" s="4">
         <v>39814</v>
       </c>
@@ -8003,7 +8022,7 @@
         <v>7.0599999427795407E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B42" s="4">
         <v>40179</v>
       </c>
@@ -8014,7 +8033,7 @@
         <v>8.7399997711181607E-2</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B43" s="4">
         <v>40544</v>
       </c>
@@ -8025,7 +8044,7 @@
         <v>8.8699998855590809E-2</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B44" s="4">
         <v>40909</v>
       </c>
@@ -8036,7 +8055,7 @@
         <v>8.8100004196166995E-2</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B45" s="4">
         <v>41275</v>
       </c>
@@ -8047,7 +8066,7 @@
         <v>9.3999996185302692E-2</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B46" s="4">
         <v>41640</v>
       </c>
@@ -8058,7 +8077,7 @@
         <v>9.92000007629395E-2</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B47" s="4">
         <v>42005</v>
       </c>
@@ -8069,7 +8088,7 @@
         <v>0.10300000190734901</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B48" s="4">
         <v>42370</v>
       </c>
@@ -8080,7 +8099,7 @@
         <v>0.103599996566772</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B49" s="4">
         <v>25569</v>
       </c>
@@ -8091,7 +8110,7 @@
         <v>2.4200000762939503E-2</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B50" s="4">
         <v>25934</v>
       </c>
@@ -8102,7 +8121,7 @@
         <v>2.6700000762939501E-2</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B51" s="4">
         <v>26299</v>
       </c>
@@ -8113,7 +8132,7 @@
         <v>2.7699999809265102E-2</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B52" s="4">
         <v>26665</v>
       </c>
@@ -8124,7 +8143,7 @@
         <v>2.69000005722046E-2</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B53" s="4">
         <v>27030</v>
       </c>
@@ -8135,7 +8154,7 @@
         <v>2.85999989509583E-2</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B54" s="4">
         <v>27395</v>
       </c>
@@ -8146,7 +8165,7 @@
         <v>4.07999992370605E-2</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B55" s="4">
         <v>27760</v>
       </c>
@@ -8157,7 +8176,7 @@
         <v>4.4699997901916505E-2</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B56" s="4">
         <v>28126</v>
       </c>
@@ -8166,7 +8185,7 @@
         <v>5.0100002288818404E-2</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B57" s="4">
         <v>28491</v>
       </c>
@@ -8177,7 +8196,7 @@
         <v>5.2699999809265104E-2</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B58" s="4">
         <v>28856</v>
       </c>
@@ -8188,7 +8207,7 @@
         <v>6.0300002098083498E-2</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B59" s="4">
         <v>29221</v>
       </c>
@@ -8199,7 +8218,7 @@
         <v>6.4200000762939496E-2</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B60" s="4">
         <v>29587</v>
       </c>
@@ -8208,7 +8227,7 @@
         <v>7.5399999618530306E-2</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B61" s="4">
         <v>29952</v>
       </c>
@@ -8219,7 +8238,7 @@
         <v>8.1999998092651405E-2</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B62" s="4">
         <v>30317</v>
       </c>
@@ -8230,7 +8249,7 @@
         <v>7.9200000762939496E-2</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B63" s="4">
         <v>30682</v>
       </c>
@@ -8241,7 +8260,7 @@
         <v>9.5299997329711894E-2</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B64" s="4">
         <v>31048</v>
       </c>
@@ -8252,7 +8271,7 @@
         <v>0.10260000228881801</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B65" s="4">
         <v>31413</v>
       </c>
@@ -8263,7 +8282,7 @@
         <v>0.102299995422363</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B66" s="4">
         <v>31778</v>
       </c>
@@ -8274,7 +8293,7 @@
         <v>0.107399997711182</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B67" s="4">
         <v>32143</v>
       </c>
@@ -8285,7 +8304,7 @@
         <v>0.10180000305175801</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B68" s="4">
         <v>32509</v>
       </c>
@@ -8296,7 +8315,7 @@
         <v>9.6199998855590801E-2</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B69" s="4">
         <v>32874</v>
       </c>
@@ -8307,7 +8326,7 @@
         <v>9.3400001525878906E-2</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B70" s="4">
         <v>33239</v>
       </c>
@@ -8318,7 +8337,7 @@
         <v>9.1300001144409199E-2</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B71" s="4">
         <v>33604</v>
       </c>
@@ -8329,7 +8348,7 @@
         <v>0.101300001144409</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B72" s="4">
         <v>33970</v>
       </c>
@@ -8340,7 +8359,7 @@
         <v>0.11199999809265099</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B73" s="4">
         <v>34335</v>
       </c>
@@ -8351,7 +8370,7 @@
         <v>0.12460000038147</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B74" s="4">
         <v>34700</v>
       </c>
@@ -8362,7 +8381,7 @@
         <v>0.118400001525879</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B75" s="4">
         <v>35065</v>
       </c>
@@ -8373,7 +8392,7 @@
         <v>0.12369999885559099</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B76" s="4">
         <v>35431</v>
       </c>
@@ -8384,7 +8403,7 @@
         <v>0.12359999656677199</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B77" s="4">
         <v>35796</v>
       </c>
@@ -8395,7 +8414,7 @@
         <v>0.118800001144409</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B78" s="4">
         <v>36161</v>
       </c>
@@ -8406,7 +8425,7 @@
         <v>0.11789999961853001</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B79" s="4">
         <v>36526</v>
       </c>
@@ -8417,7 +8436,7 @@
         <v>0.10060000419616699</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B80" s="4">
         <v>36892</v>
       </c>
@@ -8428,7 +8447,7 @@
         <v>8.819999694824221E-2</v>
       </c>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B81" s="4">
         <v>37257</v>
       </c>
@@ -8439,7 +8458,7 @@
         <v>8.9499998092651398E-2</v>
       </c>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B82" s="4">
         <v>37622</v>
       </c>
@@ -8450,7 +8469,7 @@
         <v>8.1499996185302695E-2</v>
       </c>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B83" s="4">
         <v>37987</v>
       </c>
@@ -8461,7 +8480,7 @@
         <v>8.5200004577636698E-2</v>
       </c>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B84" s="4">
         <v>38353</v>
       </c>
@@ -8472,7 +8491,7 @@
         <v>8.5000000000000006E-2</v>
       </c>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B85" s="4">
         <v>38718</v>
       </c>
@@ -8483,7 +8502,7 @@
         <v>8.4499998092651407E-2</v>
       </c>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B86" s="4">
         <v>39083</v>
       </c>
@@ -8494,7 +8513,7 @@
         <v>7.6599998474121106E-2</v>
       </c>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B87" s="4">
         <v>39448</v>
       </c>
@@ -8505,7 +8524,7 @@
         <v>7.0599999427795407E-2</v>
       </c>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B88" s="4">
         <v>39814</v>
       </c>
@@ -8516,7 +8535,7 @@
         <v>8.7399997711181607E-2</v>
       </c>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B89" s="4">
         <v>40179</v>
       </c>
@@ -8527,7 +8546,7 @@
         <v>8.8699998855590809E-2</v>
       </c>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B90" s="4">
         <v>40544</v>
       </c>
@@ -8538,7 +8557,7 @@
         <v>8.8100004196166995E-2</v>
       </c>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B91" s="4">
         <v>40909</v>
       </c>
@@ -8549,7 +8568,7 @@
         <v>9.3999996185302692E-2</v>
       </c>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B92" s="4">
         <v>41275</v>
       </c>
@@ -8560,7 +8579,7 @@
         <v>9.92000007629395E-2</v>
       </c>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B93" s="4">
         <v>41640</v>
       </c>
@@ -8571,7 +8590,7 @@
         <v>0.10300000190734901</v>
       </c>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B94" s="4">
         <v>42005</v>
       </c>
@@ -8582,7 +8601,7 @@
         <v>0.103599996566772</v>
       </c>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B95" s="4">
         <v>42370</v>
       </c>
@@ -8597,4 +8616,49 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F25CE2E-CA49-443C-BDF6-E4119F6598EF}">
+  <dimension ref="B2:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>